<commit_message>
Modify & improve README
</commit_message>
<xml_diff>
--- a/HMS-Olfactometer-v2-BOM.xlsx
+++ b/HMS-Olfactometer-v2-BOM.xlsx
@@ -138,9 +138,6 @@
     <t>up to 6 of these</t>
   </si>
   <si>
-    <t>Olfactory Delivery Box v2.0: Part List</t>
-  </si>
-  <si>
     <t>LFMX0527800B</t>
   </si>
   <si>
@@ -292,6 +289,9 @@
   </si>
   <si>
     <t>C1:  6.8µF  50V,  1812</t>
+  </si>
+  <si>
+    <t>Olfactory Delivery Box v2.0 / 2.1: Part List</t>
   </si>
 </sst>
 </file>
@@ -814,7 +814,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -828,7 +828,7 @@
   <sheetData>
     <row r="2" spans="2:9" ht="25">
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="2:9" s="2" customFormat="1">
@@ -934,7 +934,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10">
         <v>6</v>
@@ -952,13 +952,13 @@
     </row>
     <row r="11" spans="2:9">
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -1006,7 +1006,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1019,12 +1019,12 @@
         <v>33</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
@@ -1047,13 +1047,13 @@
     </row>
     <row r="21" spans="2:9">
       <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="22" spans="2:9">
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1079,13 +1079,13 @@
     </row>
     <row r="23" spans="2:9">
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1171,12 +1171,12 @@
         <v>9.1</v>
       </c>
       <c r="I31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="18">
@@ -1187,7 +1187,7 @@
         <v>17</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -1208,7 +1208,7 @@
         <v>17</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1229,7 +1229,7 @@
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -1247,7 +1247,7 @@
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1259,13 +1259,13 @@
     </row>
     <row r="38" spans="2:9">
       <c r="B38" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E38" s="10">
         <v>8</v>
@@ -1278,7 +1278,7 @@
         <v>11.44</v>
       </c>
       <c r="I38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="2:9">
@@ -1289,7 +1289,7 @@
     </row>
     <row r="40" spans="2:9">
       <c r="B40" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -1297,13 +1297,13 @@
     </row>
     <row r="41" spans="2:9">
       <c r="B41" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" s="10">
         <v>1</v>
@@ -1318,13 +1318,13 @@
     </row>
     <row r="42" spans="2:9">
       <c r="B42" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E42" s="10">
         <v>2</v>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="43" spans="2:9">
       <c r="B43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E43" s="12">
         <v>1</v>
@@ -1360,13 +1360,13 @@
     </row>
     <row r="44" spans="2:9">
       <c r="B44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" s="12">
         <v>2</v>
@@ -1381,13 +1381,13 @@
     </row>
     <row r="45" spans="2:9">
       <c r="B45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E45" s="12">
         <v>1</v>
@@ -1402,13 +1402,13 @@
     </row>
     <row r="46" spans="2:9">
       <c r="B46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E46" s="12">
         <v>2</v>
@@ -1423,13 +1423,13 @@
     </row>
     <row r="47" spans="2:9">
       <c r="B47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" t="s">
         <v>84</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" t="s">
-        <v>85</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -1442,7 +1442,7 @@
         <v>3.68</v>
       </c>
       <c r="I47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="2:9">
@@ -1452,13 +1452,13 @@
     </row>
     <row r="50" spans="2:9">
       <c r="B50" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -1473,13 +1473,13 @@
     </row>
     <row r="51" spans="2:9">
       <c r="B51" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" t="s">
         <v>71</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D51" t="s">
-        <v>72</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -1494,13 +1494,13 @@
     </row>
     <row r="52" spans="2:9">
       <c r="B52" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="53" spans="2:9">
       <c r="B53" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>17</v>
@@ -1528,18 +1528,18 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="2:9">
       <c r="B54" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -1554,13 +1554,13 @@
     </row>
     <row r="55" spans="2:9">
       <c r="B55" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -1575,13 +1575,13 @@
     </row>
     <row r="56" spans="2:9">
       <c r="B56" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -1596,10 +1596,10 @@
     </row>
     <row r="57" spans="2:9">
       <c r="B57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="2:9">

</xml_diff>

<commit_message>
[PCB] Update capacitor values; Fix silkscreen and BOM
</commit_message>
<xml_diff>
--- a/HMS-Olfactometer-v2-BOM.xlsx
+++ b/HMS-Olfactometer-v2-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
   <si>
     <t>Vendor</t>
   </si>
@@ -198,21 +198,6 @@
     <t>Advanced Circuits</t>
   </si>
   <si>
-    <t>Various resistors</t>
-  </si>
-  <si>
-    <t>C8:  1µF, 1206</t>
-  </si>
-  <si>
-    <t>C9: 1500 pF  (2kV?),  1206</t>
-  </si>
-  <si>
-    <t>C10: 2200 pF  (2kV?),  1206</t>
-  </si>
-  <si>
-    <t>C11:  4.7µF  50V,  1812</t>
-  </si>
-  <si>
     <t>We have these in shop</t>
   </si>
   <si>
@@ -228,18 +213,9 @@
     <t xml:space="preserve"> 1276-3121-1-ND</t>
   </si>
   <si>
-    <t>C5:  10µF, 50V 1206</t>
-  </si>
-  <si>
-    <t>C4:  22µF, 10V 1206</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1276-1287-1-ND</t>
   </si>
   <si>
-    <t>Might not be needed (we have in shop anyway)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 490-12457-1-ND</t>
   </si>
   <si>
@@ -288,10 +264,61 @@
     <t>Only needed if you order the Teensy 3.5 without pins</t>
   </si>
   <si>
-    <t>C1:  6.8µF  50V,  1812</t>
-  </si>
-  <si>
     <t>Olfactory Delivery Box v2.0 / 2.1: Part List</t>
+  </si>
+  <si>
+    <t>PCB Label</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>6.8µF  50V,  1812</t>
+  </si>
+  <si>
+    <t>22µF, 10V 1206</t>
+  </si>
+  <si>
+    <t>10µF, 50V 1206</t>
+  </si>
+  <si>
+    <t>1500 pF  (2kV?),  1206</t>
+  </si>
+  <si>
+    <t>2200 pF  (2kV?),  1206</t>
+  </si>
+  <si>
+    <t>4.7µF  50V,  1812</t>
+  </si>
+  <si>
+    <t>1µF, 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1276-3086-1-ND</t>
+  </si>
+  <si>
+    <t>Various thru-hole resistors</t>
+  </si>
+  <si>
+    <t>All capacitors can be exchanged for other comparable parts</t>
   </si>
 </sst>
 </file>
@@ -420,7 +447,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -434,6 +461,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -810,15 +846,16 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:I66"/>
+  <dimension ref="A2:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
+      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="10.625" style="13"/>
     <col min="2" max="2" width="23.875" customWidth="1"/>
     <col min="4" max="4" width="14.75" customWidth="1"/>
     <col min="5" max="5" width="3.875" customWidth="1"/>
@@ -826,12 +863,15 @@
     <col min="8" max="8" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="25">
+    <row r="2" spans="1:9" ht="25">
       <c r="B2" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" s="2" customFormat="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1">
+      <c r="A4" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -854,7 +894,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="1:9">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -875,7 +915,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="1:9">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -896,13 +936,13 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="1:9">
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -926,7 +966,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="1:9">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -950,7 +990,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="1:9">
       <c r="B11" t="s">
         <v>47</v>
       </c>
@@ -971,7 +1011,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="1:9">
       <c r="B12" t="s">
         <v>36</v>
       </c>
@@ -989,19 +1029,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="1:9">
       <c r="G13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="1:9">
       <c r="G14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="1:9">
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -1019,7 +1059,7 @@
         <v>33</v>
       </c>
       <c r="I15" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:9">
@@ -1171,12 +1211,12 @@
         <v>9.1</v>
       </c>
       <c r="I31" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="18">
@@ -1289,7 +1329,7 @@
     </row>
     <row r="40" spans="2:9">
       <c r="B40" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -1339,13 +1379,13 @@
     </row>
     <row r="43" spans="2:9">
       <c r="B43" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E43" s="12">
         <v>1</v>
@@ -1360,13 +1400,13 @@
     </row>
     <row r="44" spans="2:9">
       <c r="B44" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E44" s="12">
         <v>2</v>
@@ -1381,13 +1421,13 @@
     </row>
     <row r="45" spans="2:9">
       <c r="B45" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E45" s="12">
         <v>1</v>
@@ -1402,13 +1442,13 @@
     </row>
     <row r="46" spans="2:9">
       <c r="B46" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E46" s="12">
         <v>2</v>
@@ -1423,13 +1463,13 @@
     </row>
     <row r="47" spans="2:9">
       <c r="B47" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -1442,23 +1482,26 @@
         <v>3.68</v>
       </c>
       <c r="I47" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="B49" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="1:9">
+      <c r="A50" s="14" t="s">
+        <v>83</v>
+      </c>
       <c r="B50" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -1470,16 +1513,22 @@
         <f t="shared" si="1"/>
         <v>1.62</v>
       </c>
-    </row>
-    <row r="51" spans="2:9">
+      <c r="I50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="14" t="s">
+        <v>84</v>
+      </c>
       <c r="B51" s="6" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -1492,15 +1541,18 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="1:9">
+      <c r="A52" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="B52" s="6" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -1513,33 +1565,42 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="1:9">
+      <c r="A53" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="B53" s="6" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="D53" t="s">
+        <v>97</v>
+      </c>
       <c r="E53">
         <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0.14000000000000001</v>
       </c>
       <c r="G53" s="3">
         <f>E53*F53</f>
-        <v>0</v>
-      </c>
-      <c r="I53" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="14" t="s">
+        <v>87</v>
+      </c>
       <c r="B54" s="6" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -1552,15 +1613,18 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="1:9">
+      <c r="A55" s="14" t="s">
+        <v>88</v>
+      </c>
       <c r="B55" s="6" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -1573,15 +1637,18 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="1:9">
+      <c r="A56" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="B56" s="6" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -1594,15 +1661,15 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="1:9">
       <c r="B57" t="s">
+        <v>98</v>
+      </c>
+      <c r="I57" t="s">
         <v>59</v>
       </c>
-      <c r="I57" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9">
+    </row>
+    <row r="60" spans="1:9">
       <c r="B60" t="s">
         <v>27</v>
       </c>
@@ -1617,7 +1684,7 @@
     <row r="66" spans="7:7">
       <c r="G66" s="4">
         <f>SUM(G6:G65)</f>
-        <v>4675.49</v>
+        <v>4675.63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>